<commit_message>
devevelopement of the project architecture
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -1,25 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9598E700-8201-4A12-9C15-CA66BC9FE562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="ID_0001" sheetId="1" r:id="rId1"/>
+    <sheet name="ID_0002" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>automation.devmrkolv@gmail.com</t>
+  </si>
+  <si>
+    <t>$chlUe13elKiNd</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>z.</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +377,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{67CA5247-7142-4C68-86A6-E8B29C9C2871}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AF6178-9557-4C4B-AACC-CD62D3B59319}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>ID_0001!A1</f>
+        <v>USERNAME</v>
+      </c>
+      <c r="B1" t="str">
+        <f>ID_0001!B1</f>
+        <v>PASSWORD</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>ID_0001!A2</f>
+        <v>automation.devmrkolv@gmail.com</v>
+      </c>
+      <c r="B2" t="str">
+        <f>ID_0001!B2</f>
+        <v>$chlUe13elKiNd</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>ID_0001!A3</f>
+        <v>mmm</v>
+      </c>
+      <c r="B3" t="str">
+        <f>ID_0001!B3</f>
+        <v>m</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>ID_0001!A4</f>
+        <v>z.</v>
+      </c>
+      <c r="B4" t="str">
+        <f>ID_0001!B4</f>
+        <v>z</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
architecture construction: enums for configKeys, file format type by usage, further page and logic implementings. ongoing work
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9598E700-8201-4A12-9C15-CA66BC9FE562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20E54EA-2837-489F-A125-CD4C2ED6CEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID_0001" sheetId="1" r:id="rId1"/>
@@ -67,8 +67,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,8 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,10 +400,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -427,6 +436,7 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{67CA5247-7142-4C68-86A6-E8B29C9C2871}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -434,11 +444,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AF6178-9557-4C4B-AACC-CD62D3B59319}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="str">

</xml_diff>

<commit_message>
ExcelReader and ExcelActions have been set up successifully: [1] Search by Attribute; [2] Getting cell String value regardless its Celltype; [3] ExcelReader can deal with both XLS and XLSX Excel types due its calling for interfaces, not specific types (let's say: WorkBook, Sheet, Row and Cell); [4] Finally the choosen format is defined by its config.properties' previous attribuition.
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C513F3C6-A5F8-4EA2-A62F-AE0EA5D1FB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A473D8-B751-43AE-80DC-7F4C9F5C9164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3735" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID_0001" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="289">
   <si>
     <t>automation.devmrkolv@gmail.com</t>
   </si>
@@ -1242,9 +1242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1262,34 +1264,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{67CA5247-7142-4C68-86A6-E8B29C9C2871}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1383,32 +1374,32 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>ID_0001!A2</f>
-        <v>automation.devmrkolv@gmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <f>ID_0001!B2</f>
-        <v>$chlUe13elKiNd</v>
+      <c r="A2" t="e">
+        <f>ID_0001!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B2" t="e">
+        <f>ID_0001!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>ID_0001!A3</f>
+        <f>ID_0001!A2</f>
         <v>mmm</v>
       </c>
       <c r="B3" t="str">
-        <f>ID_0001!B3</f>
-        <v>m</v>
+        <f>ID_0001!B2</f>
+        <v>mmm</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>ID_0001!A4</f>
+        <f>ID_0001!A3</f>
         <v>z.</v>
       </c>
       <c r="B4" t="str">
-        <f>ID_0001!B4</f>
+        <f>ID_0001!B3</f>
         <v>z</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Preparing implementation for merge into main: [1] Class 'LoginModel' just takes it's attributes types objects for its fields; [2] So, no more Data gathering and transformations on model classes; [3] It's still needed unify path creation for parts (file or folder names, separators, etc...); [4] We must ensure that no forgotten path separator (absent or duplicated) reade from config must not interfer on data I/O at all.
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A473D8-B751-43AE-80DC-7F4C9F5C9164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593D9C07-3599-4145-8E94-577A7CD62F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3735" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ID_0001" sheetId="1" r:id="rId1"/>
-    <sheet name="ID_0002" sheetId="2" r:id="rId2"/>
-    <sheet name="ID_0003" sheetId="3" r:id="rId3"/>
-    <sheet name="ID_0004" sheetId="4" r:id="rId4"/>
-    <sheet name="ID_0005_NO_DATA_ENTITY_REQUIRED" sheetId="5" r:id="rId5"/>
-    <sheet name="ID_0006" sheetId="6" r:id="rId6"/>
-    <sheet name="ID_0007" sheetId="7" r:id="rId7"/>
-    <sheet name="ID_0008" sheetId="8" r:id="rId8"/>
-    <sheet name="ID_0009" sheetId="9" r:id="rId9"/>
-    <sheet name="ID_0010_NO_DATA_ENTITY_REQUIRED" sheetId="10" r:id="rId10"/>
-    <sheet name="ID_0011" sheetId="11" r:id="rId11"/>
-    <sheet name="ID_0012_NO_DATA_ENTITY_REQUIRED" sheetId="12" r:id="rId12"/>
+    <sheet name="USER" sheetId="12" r:id="rId1"/>
+    <sheet name="ID_0001" sheetId="1" r:id="rId2"/>
+    <sheet name="ID_0002" sheetId="2" r:id="rId3"/>
+    <sheet name="ID_0003" sheetId="3" r:id="rId4"/>
+    <sheet name="ID_0004" sheetId="4" r:id="rId5"/>
+    <sheet name="ID_0005_NO_DATA_ENTITY_REQUIRED" sheetId="5" r:id="rId6"/>
+    <sheet name="ID_0006" sheetId="6" r:id="rId7"/>
+    <sheet name="ID_0007" sheetId="7" r:id="rId8"/>
+    <sheet name="ID_0008" sheetId="8" r:id="rId9"/>
+    <sheet name="ID_0009" sheetId="9" r:id="rId10"/>
+    <sheet name="ID_0010_NO_DATA_ENTITY_REQUIRED" sheetId="10" r:id="rId11"/>
+    <sheet name="ID_0011" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,25 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="289">
-  <si>
-    <t>automation.devmrkolv@gmail.com</t>
-  </si>
-  <si>
-    <t>$chlUe13elKiNd</t>
-  </si>
-  <si>
-    <t>mmm</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>z.</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="304">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -914,13 +896,80 @@
   </si>
   <si>
     <t>EMAIL_SUFIXO</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>CREDIT_CARD_NUMBER</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>thomas3041</t>
+  </si>
+  <si>
+    <t>sandra431</t>
+  </si>
+  <si>
+    <t>0xMac2023</t>
+  </si>
+  <si>
+    <t>F391Fb&amp;#</t>
+  </si>
+  <si>
+    <t>J!H7b+TYB</t>
+  </si>
+  <si>
+    <t>3v10d3f1M</t>
+  </si>
+  <si>
+    <t>Thomas O'Donnel</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Northern Ireland</t>
+  </si>
+  <si>
+    <t>Sandra Silva da Costa</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Campo Grande</t>
+  </si>
+  <si>
+    <t>Kazuo Hatakeyama</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Sapporo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#####\ ####\ ####\ ####"/>
+    <numFmt numFmtId="165" formatCode="0####\ ####\ ####\ ####"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,6 +981,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -957,11 +1019,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,50 +1307,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8C8D86-8CDF-403E-ACE1-15E589BF149B}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F2" s="5">
+        <v>7328417382904380</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>290</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="C3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F3" s="6">
+        <v>493185717496300</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F4" s="5">
+        <f>(F3+F2)/2</f>
+        <v>3910801550200340</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687B7DD9-8B47-4BD6-8A41-4FCF0464C1C9}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57942E6E-BF9D-4681-BE2F-08D14ACCB97F}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1301,7 +1522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9876C8A2-22FE-4705-9F0E-ADF1BD8A80CA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1316,18 +1537,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" t="s">
         <v>274</v>
-      </c>
-      <c r="B2" t="s">
-        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1335,26 +1556,79 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8C8D86-8CDF-403E-ACE1-15E589BF149B}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>USER!A2</f>
+        <v>thomas3041</v>
+      </c>
+      <c r="B2" t="str">
+        <f>USER!B2</f>
+        <v>3v10d3f1M</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="str">
+        <f>USER!A3</f>
+        <v>sandra431</v>
+      </c>
+      <c r="B3" s="7" t="str">
+        <f>USER!B3</f>
+        <v>J!H7b+TYB</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="str">
+        <f>USER!A4</f>
+        <v>0xMac2023</v>
+      </c>
+      <c r="B4" s="7" t="str">
+        <f>USER!B4</f>
+        <v>F391Fb&amp;#</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AF6178-9557-4C4B-AACC-CD62D3B59319}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,43 +1638,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <f>ID_0001!A1</f>
         <v>USUARIO</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <f>ID_0001!B1</f>
         <v>SENHA</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
-        <f>ID_0001!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B2" t="e">
-        <f>ID_0001!#REF!</f>
-        <v>#REF!</v>
+      <c r="A2" t="str">
+        <f>ID_0001!A2</f>
+        <v>thomas3041</v>
+      </c>
+      <c r="B2" t="str">
+        <f>ID_0001!B2</f>
+        <v>3v10d3f1M</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>ID_0001!A2</f>
-        <v>mmm</v>
+        <f>ID_0001!A3</f>
+        <v>sandra431</v>
       </c>
       <c r="B3" t="str">
-        <f>ID_0001!B2</f>
-        <v>mmm</v>
+        <f>ID_0001!B3</f>
+        <v>J!H7b+TYB</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>ID_0001!A3</f>
-        <v>z.</v>
+        <f>ID_0001!A4</f>
+        <v>0xMac2023</v>
       </c>
       <c r="B4" t="str">
-        <f>ID_0001!B3</f>
-        <v>z</v>
+        <f>ID_0001!B4</f>
+        <v>F391Fb&amp;#</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9010A083-55DB-408F-9B8B-FD406B6AC21E}">
   <dimension ref="A1:E87"/>
   <sheetViews>
@@ -1427,986 +1701,986 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E7" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B61" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C61" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B63" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B64" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C65" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B66" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C66" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B69" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B70" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B72" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B76" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B77" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B78" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B79" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B80" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B81" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B82" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B83" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B85" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B86" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B87" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2415,12 +2689,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE47C01-D105-47BA-B3B5-EF65A81D853F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,35 +2704,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>284</v>
+      <c r="A1" s="1" t="str">
+        <f>USER!A1</f>
+        <v>USUARIO</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>USER!B1</f>
+        <v>SENHA</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="A2" s="2" t="str">
+        <f>USER!A2</f>
+        <v>thomas3041</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>USER!B2</f>
+        <v>3v10d3f1M</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="str">
+        <f>USER!A3</f>
+        <v>sandra431</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>USER!B3</f>
+        <v>J!H7b+TYB</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="A4" s="2" t="str">
+        <f>USER!A4</f>
+        <v>0xMac2023</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>USER!B4</f>
+        <v>F391Fb&amp;#</v>
       </c>
     </row>
   </sheetData>
@@ -2467,7 +2749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B9E6C9-7DE9-4CF2-A8C4-04B43D397A13}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2481,7 +2763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333CED2C-686B-4FAF-A262-DEDCD9B88E85}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2494,12 +2776,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2507,7 +2789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23770060-1CFE-45F3-A643-BA3DB83C6101}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2522,18 +2804,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2541,7 +2823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BF56A1-9B37-41BA-8328-62EBC4DA8FED}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2554,38 +2836,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687B7DD9-8B47-4BD6-8A41-4FCF0464C1C9}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scenarios from 1st until the 4th has been running successifully: [1] As Well, the Workbook 'RANDOM_GENERATED_VALUES_DATA_SET' is set for random data model geration.
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593D9C07-3599-4145-8E94-577A7CD62F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A2355-1CCF-4775-A22F-22C9C657D29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="308">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -959,6 +959,18 @@
   </si>
   <si>
     <t>Sapporo</t>
+  </si>
+  <si>
+    <t>9%!f1Fsqsrf</t>
+  </si>
+  <si>
+    <t>V@!$HQST</t>
+  </si>
+  <si>
+    <t>USUARIO_INEXISTENTE</t>
+  </si>
+  <si>
+    <t>SENHA_INEXISTENTE</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1028,6 +1040,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1560,7 +1573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
@@ -1684,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9010A083-55DB-408F-9B8B-FD406B6AC21E}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,105 +1730,98 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E2" t="s">
-        <v>239</v>
-      </c>
+      <c r="A2" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1823,863 +1829,880 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>248</v>
       </c>
       <c r="E8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B53" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C56" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C57" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C60" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C61" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C62" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B63" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C64" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B67" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C67" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>196</v>
+      </c>
+      <c r="C68" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B70" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B72" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B75" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B76" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B77" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B80" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B81" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B82" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B84" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B85" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B86" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>234</v>
+      </c>
+      <c r="B87" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>236</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2693,14 +2716,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE47C01-D105-47BA-B3B5-EF65A81D853F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2714,13 +2737,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f>USER!A2</f>
-        <v>thomas3041</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f>USER!B2</f>
-        <v>3v10d3f1M</v>
+      <c r="A2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Scenarios from 1st until the 4th has been running successifully
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593D9C07-3599-4145-8E94-577A7CD62F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A2355-1CCF-4775-A22F-22C9C657D29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="308">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -959,6 +959,18 @@
   </si>
   <si>
     <t>Sapporo</t>
+  </si>
+  <si>
+    <t>9%!f1Fsqsrf</t>
+  </si>
+  <si>
+    <t>V@!$HQST</t>
+  </si>
+  <si>
+    <t>USUARIO_INEXISTENTE</t>
+  </si>
+  <si>
+    <t>SENHA_INEXISTENTE</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1028,6 +1040,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1560,7 +1573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
@@ -1684,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9010A083-55DB-408F-9B8B-FD406B6AC21E}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,105 +1730,98 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E2" t="s">
-        <v>239</v>
-      </c>
+      <c r="A2" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1823,863 +1829,880 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>248</v>
       </c>
       <c r="E8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B53" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C56" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C57" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C60" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C61" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C62" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B63" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C64" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B67" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C67" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>196</v>
+      </c>
+      <c r="C68" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B70" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B72" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B75" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B76" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B77" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B80" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B81" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B82" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B84" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B85" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B86" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>234</v>
+      </c>
+      <c r="B87" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>236</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2693,14 +2716,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE47C01-D105-47BA-B3B5-EF65A81D853F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2714,13 +2737,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f>USER!A2</f>
-        <v>thomas3041</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f>USER!B2</f>
-        <v>3v10d3f1M</v>
+      <c r="A2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixing 4th scenario values
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A2355-1CCF-4775-A22F-22C9C657D29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B588A1E4-566E-49A6-8C0C-5DF717E39E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,10 +967,10 @@
     <t>V@!$HQST</t>
   </si>
   <si>
-    <t>USUARIO_INEXISTENTE</t>
-  </si>
-  <si>
-    <t>SENHA_INEXISTENTE</t>
+    <t>USUARIO_EXISTENTE</t>
+  </si>
+  <si>
+    <t>SENHA_EXISTENTE</t>
   </si>
 </sst>
 </file>
@@ -2717,7 +2717,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,24 +2745,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="str">
-        <f>USER!A3</f>
-        <v>sandra431</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f>USER!B3</f>
-        <v>J!H7b+TYB</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="str">
-        <f>USER!A4</f>
-        <v>0xMac2023</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f>USER!B4</f>
-        <v>F391Fb&amp;#</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
6th Scenario running sucessifully
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B588A1E4-566E-49A6-8C0C-5DF717E39E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51030A-8052-4294-8086-E5E2864CDE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="312">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -844,9 +844,6 @@
     <t>CO.JP</t>
   </si>
   <si>
-    <t>MENSAGEM</t>
-  </si>
-  <si>
     <t>Esta é uma mensagem automatizada.</t>
   </si>
   <si>
@@ -971,6 +968,21 @@
   </si>
   <si>
     <t>SENHA_EXISTENTE</t>
+  </si>
+  <si>
+    <t>CONTACT_NAME</t>
+  </si>
+  <si>
+    <t>CONTACT_MAIL</t>
+  </si>
+  <si>
+    <t>Carla Silva</t>
+  </si>
+  <si>
+    <t>carlilva@jinnmail.net</t>
+  </si>
+  <si>
+    <t>MESSAGE</t>
   </si>
 </sst>
 </file>
@@ -1323,9 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8C8D86-8CDF-403E-ACE1-15E589BF149B}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1338,45 +1348,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>287</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" t="s">
         <v>294</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2" t="s">
         <v>295</v>
-      </c>
-      <c r="D2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E2" t="s">
-        <v>296</v>
       </c>
       <c r="F2" s="5">
         <v>7328417382904380</v>
@@ -1390,19 +1400,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" t="s">
         <v>298</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>299</v>
-      </c>
-      <c r="E3" t="s">
-        <v>300</v>
       </c>
       <c r="F3" s="6">
         <v>493185717496300</v>
@@ -1416,19 +1426,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" t="s">
         <v>291</v>
       </c>
-      <c r="B4" t="s">
-        <v>292</v>
-      </c>
       <c r="C4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" t="s">
         <v>301</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>302</v>
-      </c>
-      <c r="E4" t="s">
-        <v>303</v>
       </c>
       <c r="F4" s="5">
         <f>(F3+F2)/2</f>
@@ -1507,10 +1517,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" t="s">
         <v>272</v>
-      </c>
-      <c r="B1" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1550,18 +1560,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" t="s">
         <v>275</v>
-      </c>
-      <c r="B1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1588,10 +1598,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1714,27 +1724,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2716,7 +2726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE47C01-D105-47BA-B3B5-EF65A81D853F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
@@ -2738,10 +2748,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2774,27 +2784,42 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333CED2C-686B-4FAF-A262-DEDCD9B88E85}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2813,18 +2838,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" t="s">
         <v>268</v>
-      </c>
-      <c r="B2" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2845,12 +2870,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scenario ID_0007 running successifully: although implicit waits are needed then. replace it with some 'jsWait' or 'flagWebElementWait'
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51030A-8052-4294-8086-E5E2864CDE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCFEC0A-C4AA-4432-B6D8-431AEE16693F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="313">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -853,136 +853,139 @@
     <t>Laptops</t>
   </si>
   <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>Monitors</t>
+  </si>
+  <si>
+    <t>PRODUTO_1</t>
+  </si>
+  <si>
+    <t>PRODUTO_2</t>
+  </si>
+  <si>
+    <t>Phones</t>
+  </si>
+  <si>
+    <t>CATEGORY_1</t>
+  </si>
+  <si>
+    <t>CATEGORY_2</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>SENHA</t>
+  </si>
+  <si>
+    <t>NOME_MASCULINO</t>
+  </si>
+  <si>
+    <t>NOME_FEMININO</t>
+  </si>
+  <si>
+    <t>EMAIL_EMPRESA</t>
+  </si>
+  <si>
+    <t>EMAIL_SUFIXO</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>CREDIT_CARD_NUMBER</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>thomas3041</t>
+  </si>
+  <si>
+    <t>sandra431</t>
+  </si>
+  <si>
+    <t>0xMac2023</t>
+  </si>
+  <si>
+    <t>F391Fb&amp;#</t>
+  </si>
+  <si>
+    <t>J!H7b+TYB</t>
+  </si>
+  <si>
+    <t>3v10d3f1M</t>
+  </si>
+  <si>
+    <t>Thomas O'Donnel</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Northern Ireland</t>
+  </si>
+  <si>
+    <t>Sandra Silva da Costa</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Campo Grande</t>
+  </si>
+  <si>
+    <t>Kazuo Hatakeyama</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Sapporo</t>
+  </si>
+  <si>
+    <t>9%!f1Fsqsrf</t>
+  </si>
+  <si>
+    <t>V@!$HQST</t>
+  </si>
+  <si>
+    <t>USUARIO_EXISTENTE</t>
+  </si>
+  <si>
+    <t>SENHA_EXISTENTE</t>
+  </si>
+  <si>
+    <t>CONTACT_NAME</t>
+  </si>
+  <si>
+    <t>CONTACT_MAIL</t>
+  </si>
+  <si>
+    <t>Carla Silva</t>
+  </si>
+  <si>
+    <t>carlilva@jinnmail.net</t>
+  </si>
+  <si>
+    <t>MESSAGE</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
     <t>Dell</t>
-  </si>
-  <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>Monitors</t>
-  </si>
-  <si>
-    <t>PRODUTO_1</t>
-  </si>
-  <si>
-    <t>PRODUTO_2</t>
-  </si>
-  <si>
-    <t>Phones</t>
-  </si>
-  <si>
-    <t>CATEGORY_1</t>
-  </si>
-  <si>
-    <t>CATEGORY_2</t>
-  </si>
-  <si>
-    <t>USUARIO</t>
-  </si>
-  <si>
-    <t>SENHA</t>
-  </si>
-  <si>
-    <t>NOME_MASCULINO</t>
-  </si>
-  <si>
-    <t>NOME_FEMININO</t>
-  </si>
-  <si>
-    <t>EMAIL_EMPRESA</t>
-  </si>
-  <si>
-    <t>EMAIL_SUFIXO</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>COUNTRY</t>
-  </si>
-  <si>
-    <t>CITY</t>
-  </si>
-  <si>
-    <t>CREDIT_CARD_NUMBER</t>
-  </si>
-  <si>
-    <t>MONTH</t>
-  </si>
-  <si>
-    <t>YEAR</t>
-  </si>
-  <si>
-    <t>thomas3041</t>
-  </si>
-  <si>
-    <t>sandra431</t>
-  </si>
-  <si>
-    <t>0xMac2023</t>
-  </si>
-  <si>
-    <t>F391Fb&amp;#</t>
-  </si>
-  <si>
-    <t>J!H7b+TYB</t>
-  </si>
-  <si>
-    <t>3v10d3f1M</t>
-  </si>
-  <si>
-    <t>Thomas O'Donnel</t>
-  </si>
-  <si>
-    <t>Belfast</t>
-  </si>
-  <si>
-    <t>Northern Ireland</t>
-  </si>
-  <si>
-    <t>Sandra Silva da Costa</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Campo Grande</t>
-  </si>
-  <si>
-    <t>Kazuo Hatakeyama</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Sapporo</t>
-  </si>
-  <si>
-    <t>9%!f1Fsqsrf</t>
-  </si>
-  <si>
-    <t>V@!$HQST</t>
-  </si>
-  <si>
-    <t>USUARIO_EXISTENTE</t>
-  </si>
-  <si>
-    <t>SENHA_EXISTENTE</t>
-  </si>
-  <si>
-    <t>CONTACT_NAME</t>
-  </si>
-  <si>
-    <t>CONTACT_MAIL</t>
-  </si>
-  <si>
-    <t>Carla Silva</t>
-  </si>
-  <si>
-    <t>carlilva@jinnmail.net</t>
-  </si>
-  <si>
-    <t>MESSAGE</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8C8D86-8CDF-403E-ACE1-15E589BF149B}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1348,45 +1351,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" t="s">
         <v>293</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" t="s">
         <v>294</v>
-      </c>
-      <c r="D2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E2" t="s">
-        <v>295</v>
       </c>
       <c r="F2" s="5">
         <v>7328417382904380</v>
@@ -1400,19 +1403,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" t="s">
         <v>297</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>298</v>
-      </c>
-      <c r="E3" t="s">
-        <v>299</v>
       </c>
       <c r="F3" s="6">
         <v>493185717496300</v>
@@ -1426,19 +1429,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" t="s">
         <v>290</v>
       </c>
-      <c r="B4" t="s">
-        <v>291</v>
-      </c>
       <c r="C4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" t="s">
         <v>300</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>301</v>
-      </c>
-      <c r="E4" t="s">
-        <v>302</v>
       </c>
       <c r="F4" s="5">
         <f>(F3+F2)/2</f>
@@ -1517,10 +1520,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" t="s">
-        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -1560,10 +1563,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" t="s">
         <v>274</v>
-      </c>
-      <c r="B1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1574,7 @@
         <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -1598,10 +1601,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1724,27 +1727,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2748,10 +2751,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2797,21 +2800,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" t="s">
         <v>309</v>
-      </c>
-      <c r="B2" t="s">
-        <v>310</v>
       </c>
       <c r="C2" t="s">
         <v>265</v>
@@ -2825,35 +2828,50 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23770060-1CFE-45F3-A643-BA3DB83C6101}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>ID_0001!A1</f>
+        <v>USUARIO</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>ID_0001!B1</f>
+        <v>SENHA</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B2" t="s">
-        <v>268</v>
+      <c r="D2" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2875,7 +2893,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting the 8th scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCFEC0A-C4AA-4432-B6D8-431AEE16693F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6BDCD0-9A21-4175-8444-F91EB0DCCB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3585" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="ID_0011" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="315">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -986,6 +987,12 @@
   </si>
   <si>
     <t>Dell</t>
+  </si>
+  <si>
+    <t>CATEGORIA_1</t>
+  </si>
+  <si>
+    <t>CATEGORIA_2</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687B7DD9-8B47-4BD6-8A41-4FCF0464C1C9}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,12 +1525,28 @@
     <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>ID_0001!A1</f>
+        <v>USUARIO</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>ID_0001!B1</f>
+        <v>SENHA</v>
+      </c>
+      <c r="C1" t="s">
         <v>270</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2830,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23770060-1CFE-45F3-A643-BA3DB83C6101}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,23 +2900,45 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BF56A1-9B37-41BA-8328-62EBC4DA8FED}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>ID_0001!A1</f>
+        <v>USUARIO</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>ID_0001!B1</f>
+        <v>SENHA</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" t="s">
         <v>269</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scenario for ID_0008 has been working successifully
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6BDCD0-9A21-4175-8444-F91EB0DCCB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECFED92-1CE1-4E31-B090-05A3A92FE6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3585" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,6 @@
     <sheet name="ID_0011" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -986,13 +985,13 @@
     <t>mmm</t>
   </si>
   <si>
-    <t>Dell</t>
-  </si>
-  <si>
     <t>CATEGORIA_1</t>
   </si>
   <si>
     <t>CATEGORIA_2</t>
+  </si>
+  <si>
+    <t>Sony</t>
   </si>
 </sst>
 </file>
@@ -2853,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23770060-1CFE-45F3-A643-BA3DB83C6101}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,7 +2888,7 @@
         <v>267</v>
       </c>
       <c r="D2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +2901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BF56A1-9B37-41BA-8328-62EBC4DA8FED}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2921,10 +2920,10 @@
         <v>SENHA</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
features' name have been padronized
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECFED92-1CE1-4E31-B090-05A3A92FE6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D1A9C0-E240-4EBC-AEC6-DCE82C8C0599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="313">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -857,12 +857,6 @@
   </si>
   <si>
     <t>Monitors</t>
-  </si>
-  <si>
-    <t>PRODUTO_1</t>
-  </si>
-  <si>
-    <t>PRODUTO_2</t>
   </si>
   <si>
     <t>Phones</t>
@@ -1357,45 +1351,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E2" t="s">
         <v>292</v>
-      </c>
-      <c r="C2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E2" t="s">
-        <v>294</v>
       </c>
       <c r="F2" s="5">
         <v>7328417382904380</v>
@@ -1409,19 +1403,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E3" t="s">
         <v>296</v>
-      </c>
-      <c r="D3" t="s">
-        <v>297</v>
-      </c>
-      <c r="E3" t="s">
-        <v>298</v>
       </c>
       <c r="F3" s="6">
         <v>493185717496300</v>
@@ -1435,19 +1429,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E4" t="s">
         <v>299</v>
-      </c>
-      <c r="D4" t="s">
-        <v>300</v>
-      </c>
-      <c r="E4" t="s">
-        <v>301</v>
       </c>
       <c r="F4" s="5">
         <f>(F3+F2)/2</f>
@@ -1515,13 +1509,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687B7DD9-8B47-4BD6-8A41-4FCF0464C1C9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1533,19 +1528,25 @@
         <f>ID_0001!B1</f>
         <v>SENHA</v>
       </c>
-      <c r="C1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D1" t="s">
-        <v>271</v>
+      <c r="C1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
+      </c>
+      <c r="C2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1585,10 +1586,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1596,7 +1597,7 @@
         <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1623,10 +1624,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1749,27 +1750,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2773,10 +2774,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2822,21 +2823,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C2" t="s">
         <v>265</v>
@@ -2852,7 +2853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23770060-1CFE-45F3-A643-BA3DB83C6101}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2879,16 +2880,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>267</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +2903,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2920,18 +2921,18 @@
         <v>SENHA</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C2" t="s">
         <v>269</v>

</xml_diff>

<commit_message>
scenario 8 fix finished
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D1A9C0-E240-4EBC-AEC6-DCE82C8C0599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D2808-899D-4681-B793-A7DB4906E81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="313">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -1509,14 +1509,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687B7DD9-8B47-4BD6-8A41-4FCF0464C1C9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2902,13 +2902,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BF56A1-9B37-41BA-8328-62EBC4DA8FED}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2921,11 +2922,9 @@
         <v>SENHA</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>311</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2936,9 +2935,6 @@
       </c>
       <c r="C2" t="s">
         <v>269</v>
-      </c>
-      <c r="D2" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finishing 10th scenario skeleton
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D2808-899D-4681-B793-A7DB4906E81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E398499-3C4B-46A4-8847-90CB070E0EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7785" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="ID_0007" sheetId="7" r:id="rId8"/>
     <sheet name="ID_0008" sheetId="8" r:id="rId9"/>
     <sheet name="ID_0009" sheetId="9" r:id="rId10"/>
-    <sheet name="ID_0010_NO_DATA_ENTITY_REQUIRED" sheetId="10" r:id="rId11"/>
+    <sheet name="ID_0010" sheetId="10" r:id="rId11"/>
     <sheet name="ID_0011" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="313">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -1510,7 +1510,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,17 +1556,48 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57942E6E-BF9D-4681-BE2F-08D14ACCB97F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>ID_0001!A1</f>
+        <v>USUARIO</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>ID_0001!B1</f>
+        <v>SENHA</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -2902,7 +2933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BF56A1-9B37-41BA-8328-62EBC4DA8FED}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
scenario 11 working sucessifully
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E398499-3C4B-46A4-8847-90CB070E0EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4702C29-3D67-4BBC-9613-4714206A8342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7785" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="15375" windowHeight="7785" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="310">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -857,15 +857,6 @@
   </si>
   <si>
     <t>Monitors</t>
-  </si>
-  <si>
-    <t>Phones</t>
-  </si>
-  <si>
-    <t>CATEGORY_1</t>
-  </si>
-  <si>
-    <t>CATEGORY_2</t>
   </si>
   <si>
     <t>USUARIO</t>
@@ -1351,45 +1342,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>281</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2" t="s">
         <v>290</v>
       </c>
-      <c r="C2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D2" t="s">
-        <v>293</v>
-      </c>
       <c r="E2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F2" s="5">
         <v>7328417382904380</v>
@@ -1403,19 +1394,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3" t="s">
         <v>286</v>
       </c>
-      <c r="B3" t="s">
-        <v>289</v>
-      </c>
       <c r="C3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F3" s="6">
         <v>493185717496300</v>
@@ -1429,19 +1420,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F4" s="5">
         <f>(F3+F2)/2</f>
@@ -1529,18 +1520,18 @@
         <v>SENHA</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C2" t="s">
         <v>269</v>
@@ -1558,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57942E6E-BF9D-4681-BE2F-08D14ACCB97F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,18 +1568,18 @@
         <v>SENHA</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C2" t="s">
         <v>269</v>
@@ -1604,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9876C8A2-22FE-4705-9F0E-ADF1BD8A80CA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,20 +1606,34 @@
     <col min="1" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>ID_0001!A1</f>
+        <v>USUARIO</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>ID_0001!B1</f>
+        <v>SENHA</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" t="s">
         <v>267</v>
-      </c>
-      <c r="B2" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1655,10 +1660,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1781,27 +1786,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2805,10 +2810,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2854,21 +2859,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C2" t="s">
         <v>265</v>
@@ -2911,16 +2916,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>267</v>
       </c>
       <c r="D2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2959,10 +2964,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C2" t="s">
         <v>269</v>

</xml_diff>

<commit_message>
skeleton for scenario 12 has been finished
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4702C29-3D67-4BBC-9613-4714206A8342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC4FACB-F6F4-42A9-A7DF-EF51D7FF3DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="15375" windowHeight="7785" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="ID_0009" sheetId="9" r:id="rId10"/>
     <sheet name="ID_0010" sheetId="10" r:id="rId11"/>
     <sheet name="ID_0011" sheetId="11" r:id="rId12"/>
+    <sheet name="ID_0012" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="317">
   <si>
     <t>SOBRENOME</t>
   </si>
@@ -977,6 +978,27 @@
   </si>
   <si>
     <t>Sony</t>
+  </si>
+  <si>
+    <t>Phones</t>
+  </si>
+  <si>
+    <t>CREDIT_CARD_EXP_MONTH</t>
+  </si>
+  <si>
+    <t>CREDIT_CARD_EXP_YEAR</t>
+  </si>
+  <si>
+    <t>Günther Gottlieb</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Rostock</t>
+  </si>
+  <si>
+    <t>8539-9538-0492-0428</t>
   </si>
 </sst>
 </file>
@@ -1017,12 +1039,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1037,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1047,6 +1075,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1597,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9876C8A2-22FE-4705-9F0E-ADF1BD8A80CA}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -1635,6 +1665,97 @@
       <c r="D2" t="s">
         <v>267</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D081ED5-08DE-454B-984F-C188E389548E}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>ID_0001!A1</f>
+        <v>USUARIO</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>ID_0001!B1</f>
+        <v>SENHA</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="10">
+        <v>12</v>
+      </c>
+      <c r="J2" s="10">
+        <v>30</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
we still need validate the sum
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SET.xlsx
+++ b/src/main/resources/DATA_SET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\AVALIACOES_KEEGGO\AVALIACAO_02_DEMOBLAZE\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC4FACB-F6F4-42A9-A7DF-EF51D7FF3DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBFF708-187D-4F2F-B5EC-5283B9B84E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="12" r:id="rId1"/>
@@ -1579,7 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57942E6E-BF9D-4681-BE2F-08D14ACCB97F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -1628,7 +1628,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,10 +1660,10 @@
         <v>306</v>
       </c>
       <c r="C2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
-        <v>267</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -1675,7 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D081ED5-08DE-454B-984F-C188E389548E}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>